<commit_message>
se sube proyecto de automatización y modificaciones en los test cases
</commit_message>
<xml_diff>
--- a/Documents/TestCases.xlsx
+++ b/Documents/TestCases.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YilmerD\QAA\VoloteaFront\VoloteaFront\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C1AFA7-050B-4C48-8A60-C93F602BD96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C4AC87-E894-477F-9430-BE6F707AE090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{C3F1010C-58CB-4765-AD2A-102353A66524}"/>
   </bookViews>
   <sheets>
     <sheet name="BUSCADOR DE PASAJEROS" sheetId="1" r:id="rId1"/>
     <sheet name="BUSCADOR ORIGEN" sheetId="2" r:id="rId2"/>
+    <sheet name="AUTOMATIZAR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="67">
   <si>
     <t>No.</t>
   </si>
@@ -159,9 +160,6 @@
     <t>TC-P08</t>
   </si>
   <si>
-    <t xml:space="preserve">Si se dismuneye la cantidad de adultos a 0, los bebés se deben bloquear </t>
-  </si>
-  <si>
     <t>Si se selecciona más de 9 adultos se debe mostrar una alerta con un link que direcciona a "Reserva de grupos", abajo de Adultos</t>
   </si>
   <si>
@@ -456,18 +454,12 @@
     </r>
   </si>
   <si>
-    <t>Si selecciona la opción Países, se debe mostar unas cajas con los paises que tiene presencia la aerolinea y la cantidad de ciudades donde opera.</t>
-  </si>
-  <si>
     <t>En la parte inferior mostrar las ciudades agrupadas por país, según el país seleccionado</t>
   </si>
   <si>
     <t xml:space="preserve"> Si selecciona la opción Ciudades, se debe mostrar agrupada por países las ciudades donde opera</t>
   </si>
   <si>
-    <t xml:space="preserve"> Al seleccionar una ciudad se debe expandir el campo destino (los destinos disponibles para la ciudad seleccionada)</t>
-  </si>
-  <si>
     <t>Al hacer click sobre el campo origen se debe permitir borrar lo seleccionado y buscar por nombre o código IATA</t>
   </si>
   <si>
@@ -678,6 +670,61 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> tener otras opciones de busqueda</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Si se disminuye la cantidad de adultos a 0, los bebés se deben bloquear </t>
+  </si>
+  <si>
+    <t>BUSCADOR PASAJEROS</t>
+  </si>
+  <si>
+    <t>COMO Pasajero
+QUIERO Seleccionar la cantidad de pasajeros
+PARA Indicar la cantidad de personas que viajan conmigo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2. Dar clic en el radio button de 1 pasajero. Por defecto estará preseleccionado 1 adulto.   </t>
+  </si>
+  <si>
+    <t>1. Ir a la URL https://www.volotea.com/es/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   3. Seleccionar 6 Adultos y  6 bebés, dando clic en el botón de (+) en cada uno de ellos</t>
+  </si>
+  <si>
+    <t>then he can see an adult preselected</t>
+  </si>
+  <si>
+    <t>when you click on passenger</t>
+  </si>
+  <si>
+    <t>given the user in the search section</t>
+  </si>
+  <si>
+    <t>Si selecciona la opción Países, se debe mostrar unas cajas con los paises que tiene presencia la aerolinea y la cantidad de ciudades donde opera.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Al seleccionar una ciudad se debe expandir el campo destino</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (los destinos disponibles para la ciudad seleccionada)</t>
     </r>
   </si>
 </sst>
@@ -776,7 +823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -805,40 +852,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1157,8 +1198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4AB58E-A29F-4B85-94BC-F2D3BA1C081B}">
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1208,7 @@
     <col min="2" max="2" width="24" style="2" customWidth="1"/>
     <col min="3" max="3" width="56.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="44.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="20.140625" style="2" customWidth="1"/>
     <col min="7" max="7" width="38" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.28515625" style="2" customWidth="1"/>
@@ -1211,923 +1252,988 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>15</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="18"/>
+      <c r="K2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="F3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="18"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="F4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
+      <c r="F6" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="17"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="11" t="s">
+      <c r="D8" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="11"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="6"/>
-    </row>
-    <row r="7" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8" t="s">
+      <c r="H8" s="3"/>
+      <c r="I8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="6"/>
-    </row>
-    <row r="8" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="10" t="s">
+      <c r="D11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="s">
+      <c r="F13" s="6"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="11" t="s">
+      <c r="D14" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="6"/>
-      <c r="I11" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="8" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J14" s="18"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A15" s="19"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="6"/>
+      <c r="I17" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="16"/>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
+      <c r="F18" s="6"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="3"/>
-      <c r="I14" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" s="10"/>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A16" s="12"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8" t="s">
+      <c r="D20" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="11"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="11" t="s">
+      <c r="F20" s="3"/>
+      <c r="G20" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="6"/>
-      <c r="I17" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="11"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="s">
+      <c r="H20" s="3"/>
+      <c r="I20" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="J20" s="18"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D19" s="11"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5" t="s">
+      <c r="F21" s="3"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="10"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="10" t="s">
+      <c r="D23" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J20" s="10"/>
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
+      <c r="H23" s="6"/>
+      <c r="I23" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="16"/>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" ht="33" x14ac:dyDescent="0.25">
+      <c r="A24" s="17"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="6"/>
-      <c r="I23" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J23" s="11"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="8" t="s">
+      <c r="F24" s="6"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="6"/>
+    </row>
+    <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="11"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="11"/>
+      <c r="G25" s="16"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
+      <c r="A26" s="10"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="14"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-      <c r="K27" s="14"/>
+      <c r="A27" s="10"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="14"/>
+      <c r="A28" s="10"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
     </row>
     <row r="29" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-      <c r="K29" s="14"/>
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
     </row>
     <row r="30" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-      <c r="K30" s="14"/>
+      <c r="A30" s="10"/>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
     </row>
     <row r="31" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
-      <c r="B31" s="14"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-      <c r="K31" s="14"/>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
     </row>
     <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="14"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
     </row>
     <row r="33" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-      <c r="K33" s="14"/>
+      <c r="A33" s="10"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
     </row>
     <row r="34" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
+      <c r="A34" s="10"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
     </row>
     <row r="35" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
+      <c r="A35" s="10"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
     </row>
     <row r="36" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
+      <c r="A36" s="10"/>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
     </row>
     <row r="37" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
+      <c r="A37" s="10"/>
+      <c r="B37" s="10"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="G37" s="10"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
     </row>
     <row r="38" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-      <c r="K38" s="14"/>
+      <c r="A38" s="10"/>
+      <c r="B38" s="10"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="10"/>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
     </row>
     <row r="39" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="14"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
+      <c r="A39" s="10"/>
+      <c r="B39" s="10"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
     </row>
     <row r="40" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="14"/>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-      <c r="K40" s="14"/>
+      <c r="A40" s="10"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="10"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
     </row>
     <row r="41" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="14"/>
-      <c r="B41" s="14"/>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
+      <c r="A41" s="10"/>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="10"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
     </row>
     <row r="42" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
-      <c r="B42" s="14"/>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-      <c r="K42" s="14"/>
+      <c r="A42" s="10"/>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
     </row>
     <row r="43" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
-      <c r="B43" s="14"/>
-      <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+      <c r="K43" s="10"/>
     </row>
     <row r="44" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-      <c r="K44" s="14"/>
+      <c r="A44" s="10"/>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+      <c r="K44" s="10"/>
     </row>
     <row r="45" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
-      <c r="B45" s="14"/>
-      <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
+      <c r="A45" s="10"/>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
+      <c r="J45" s="10"/>
+      <c r="K45" s="10"/>
     </row>
     <row r="46" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
-      <c r="B46" s="14"/>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
+      <c r="A46" s="10"/>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="10"/>
+      <c r="K46" s="10"/>
     </row>
     <row r="47" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
+      <c r="A47" s="10"/>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="10"/>
+      <c r="F47" s="10"/>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="10"/>
+      <c r="J47" s="10"/>
+      <c r="K47" s="10"/>
     </row>
     <row r="48" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
+      <c r="A48" s="10"/>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
     </row>
     <row r="49" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
-      <c r="B49" s="14"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="10"/>
+      <c r="J49" s="10"/>
+      <c r="K49" s="10"/>
     </row>
     <row r="50" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-      <c r="K50" s="14"/>
+      <c r="A50" s="10"/>
+      <c r="B50" s="10"/>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="10"/>
     </row>
     <row r="51" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
+      <c r="A51" s="10"/>
+      <c r="B51" s="10"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="10"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="10"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10"/>
     </row>
     <row r="52" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="14"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
+      <c r="A52" s="10"/>
+      <c r="B52" s="10"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
     </row>
     <row r="53" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="14"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-      <c r="K53" s="14"/>
+      <c r="A53" s="10"/>
+      <c r="B53" s="10"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
     </row>
     <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
+      <c r="A54" s="10"/>
+      <c r="B54" s="10"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
     </row>
     <row r="55" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-      <c r="K55" s="14"/>
+      <c r="A55" s="10"/>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="10"/>
     </row>
     <row r="56" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
+      <c r="A56" s="10"/>
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="10"/>
     </row>
     <row r="57" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
+      <c r="A57" s="10"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="10"/>
     </row>
     <row r="58" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
-      <c r="B58" s="14"/>
-      <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
+      <c r="A58" s="10"/>
+      <c r="B58" s="10"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="10"/>
     </row>
     <row r="59" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
-      <c r="B59" s="14"/>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-      <c r="K59" s="14"/>
+      <c r="A59" s="10"/>
+      <c r="B59" s="10"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
+      <c r="J59" s="10"/>
+      <c r="K59" s="10"/>
     </row>
     <row r="60" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
-      <c r="B60" s="14"/>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-      <c r="K60" s="14"/>
+      <c r="A60" s="10"/>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
     </row>
     <row r="61" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
-      <c r="B61" s="14"/>
-      <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-      <c r="K61" s="14"/>
+      <c r="A61" s="10"/>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="10"/>
+      <c r="I61" s="10"/>
+      <c r="J61" s="10"/>
+      <c r="K61" s="10"/>
     </row>
     <row r="62" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
-      <c r="B62" s="14"/>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
+      <c r="A62" s="10"/>
+      <c r="B62" s="10"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10"/>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="10"/>
+      <c r="K62" s="10"/>
     </row>
     <row r="63" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
-      <c r="B63" s="14"/>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-      <c r="K63" s="14"/>
+      <c r="A63" s="10"/>
+      <c r="B63" s="10"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="10"/>
+      <c r="E63" s="10"/>
+      <c r="F63" s="10"/>
+      <c r="G63" s="10"/>
+      <c r="H63" s="10"/>
+      <c r="I63" s="10"/>
+      <c r="J63" s="10"/>
+      <c r="K63" s="10"/>
     </row>
     <row r="64" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
-      <c r="B64" s="14"/>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-      <c r="K64" s="14"/>
+      <c r="A64" s="10"/>
+      <c r="B64" s="10"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10"/>
+      <c r="F64" s="10"/>
+      <c r="G64" s="10"/>
+      <c r="H64" s="10"/>
+      <c r="I64" s="10"/>
+      <c r="J64" s="10"/>
+      <c r="K64" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="48">
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="J23:J25"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="J2:J4"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J14:J16"/>
     <mergeCell ref="I20:I22"/>
     <mergeCell ref="I23:I25"/>
     <mergeCell ref="I5:I7"/>
@@ -2135,6 +2241,15 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="I14:I16"/>
     <mergeCell ref="I17:I19"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="C17:C19"/>
     <mergeCell ref="D23:D25"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="G23:G25"/>
@@ -2151,23 +2266,13 @@
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="G5:G7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="J2:J4"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="J23:J25"/>
-    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2180,7 +2285,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G2" sqref="G2:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,18 +2338,18 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="10" t="s">
-        <v>44</v>
+      <c r="G2" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -2252,48 +2357,48 @@
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="99" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="10"/>
+        <v>46</v>
+      </c>
+      <c r="D3" s="18"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="10"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="D4" s="18"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="10"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="16"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-      <c r="G5" s="11" t="s">
-        <v>45</v>
+      <c r="G5" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -2301,37 +2406,37 @@
       <c r="K5" s="6"/>
     </row>
     <row r="6" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="7"/>
       <c r="C6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="11"/>
+        <v>48</v>
+      </c>
+      <c r="D6" s="16"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="11"/>
+      <c r="G6" s="16"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="7"/>
       <c r="C7" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="11"/>
+        <v>49</v>
+      </c>
+      <c r="D7" s="16"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="11"/>
+      <c r="G7" s="16"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
     </row>
     <row r="8" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="4"/>
@@ -2341,8 +2446,8 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="10" t="s">
-        <v>46</v>
+      <c r="G8" s="18" t="s">
+        <v>44</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -2350,37 +2455,37 @@
       <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
-      <c r="G9" s="10"/>
+      <c r="G9" s="18"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="18"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
-      <c r="G10" s="10"/>
+      <c r="G10" s="18"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
     <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="7"/>
@@ -2390,8 +2495,8 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="11" t="s">
-        <v>47</v>
+      <c r="G11" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -2399,37 +2504,37 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="7"/>
       <c r="C12" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="11"/>
+      <c r="G12" s="16"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="11"/>
+      <c r="G13" s="16"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="18" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="4"/>
@@ -2439,8 +2544,8 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="10" t="s">
-        <v>48</v>
+      <c r="G14" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2448,190 +2553,190 @@
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:11" ht="99" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="10"/>
+      <c r="G15" s="18"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="33" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="18"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="21"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="19"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="21"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
     </row>
     <row r="23" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="21"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
     </row>
     <row r="28" spans="1:11" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2649,5 +2754,20 @@
     <mergeCell ref="D5:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7C605BF-E966-4079-91C8-66B4393A13B8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se actualiza automatización DepartureDate
</commit_message>
<xml_diff>
--- a/Documents/TestCases.xlsx
+++ b/Documents/TestCases.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="775" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="775" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BUSCADOR DE PASAJEROS" sheetId="1" r:id="rId1"/>
     <sheet name="BUSCADOR ORIGEN" sheetId="2" r:id="rId2"/>
-    <sheet name="DESTINO" sheetId="6" r:id="rId3"/>
+    <sheet name="BUSCADOR DESTINO" sheetId="6" r:id="rId3"/>
     <sheet name="BUSCADOR FECHA IDA" sheetId="5" r:id="rId4"/>
     <sheet name="BUSCADOR FECHA REGRESO" sheetId="4" r:id="rId5"/>
     <sheet name="AUTOMATIZAR" sheetId="3" r:id="rId6"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="137">
   <si>
     <t>Indentificador</t>
   </si>
@@ -965,9 +965,6 @@
     <t>COMO Pasajero   QUIERO Seleccionar el destino PARA Indicar el hasta donde quiero dirigirme</t>
   </si>
   <si>
-    <t>1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Origen en el buscador de viajes                             3. Seleccionar pestaña Country</t>
-  </si>
-  <si>
     <t>BUSCADOR FECHA IDA</t>
   </si>
   <si>
@@ -1061,6 +1058,22 @@
   </si>
   <si>
     <t>Si se selecciona una fecha y la fecha de origen la cambio por una posterior a la fecha de vuelta, la fecha de vuelta se debe eliminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Destino en el buscador de viajes        </t>
+  </si>
+  <si>
+    <t>Feature: DestinationCity
+  As QA Automation
+  I want to enter in selector Destination
+  To validate selector Destination
+  Background: Select Selector Destination
+    Given The user in the search section
+  Scenario:Select Selector Destination
+    When this user clicks on destination city
+    Then he can see the destination cities the user can travel to ESPAÑA
+When this user clicks on city of origin
+Then he can select a city from the list of origin cities</t>
   </si>
 </sst>
 </file>
@@ -3430,8 +3443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3445,7 +3458,7 @@
     <col min="7" max="7" width="32.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="42.7109375" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -3495,7 +3508,7 @@
         <v>118</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="F2" s="56" t="s">
         <v>110</v>
@@ -3507,8 +3520,8 @@
       <c r="I2" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="28" t="s">
-        <v>92</v>
+      <c r="J2" s="31" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
@@ -3523,9 +3536,9 @@
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="1:10" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="43"/>
       <c r="C4" s="30"/>
@@ -3537,7 +3550,7 @@
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
@@ -4389,8 +4402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4404,7 +4417,7 @@
     <col min="7" max="7" width="32.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -4440,15 +4453,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45" t="s">
         <v>113</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>10</v>
@@ -4457,7 +4470,7 @@
         <v>85</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="28" t="s">
@@ -4466,47 +4479,47 @@
       <c r="I2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J2" s="31" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="45"/>
       <c r="B3" s="38"/>
       <c r="C3" s="29"/>
       <c r="D3" s="67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
       <c r="H3" s="29"/>
       <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="1:10" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="45"/>
       <c r="B4" s="43"/>
       <c r="C4" s="30"/>
       <c r="D4" s="68" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>114</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>10</v>
@@ -4515,7 +4528,7 @@
         <v>85</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25" t="s">
@@ -4559,10 +4572,10 @@
         <v>115</v>
       </c>
       <c r="B8" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
@@ -4571,7 +4584,7 @@
         <v>85</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G8" s="28"/>
       <c r="H8" s="28" t="s">
@@ -5341,8 +5354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G7"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5397,7 +5410,7 @@
         <v>116</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>38</v>
@@ -5409,7 +5422,7 @@
         <v>85</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G2" s="28"/>
       <c r="H2" s="28" t="s">
@@ -5427,7 +5440,7 @@
       <c r="B3" s="38"/>
       <c r="C3" s="29"/>
       <c r="D3" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" s="32"/>
       <c r="F3" s="29"/>
@@ -5441,7 +5454,7 @@
       <c r="B4" s="43"/>
       <c r="C4" s="30"/>
       <c r="D4" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E4" s="33"/>
       <c r="F4" s="30"/>
@@ -5455,19 +5468,19 @@
         <v>117</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C5" s="25" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E5" s="34" t="s">
         <v>85</v>
       </c>
       <c r="F5" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" s="25"/>
       <c r="H5" s="25" t="s">
@@ -5483,7 +5496,7 @@
       <c r="B6" s="40"/>
       <c r="C6" s="26"/>
       <c r="D6" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E6" s="35"/>
       <c r="F6" s="26"/>
@@ -5497,7 +5510,7 @@
       <c r="B7" s="40"/>
       <c r="C7" s="27"/>
       <c r="D7" s="16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E7" s="36"/>
       <c r="F7" s="27"/>

</xml_diff>

<commit_message>
se actualiza automatización ReturnDate y se realiza reporte final de las automatizaciones
</commit_message>
<xml_diff>
--- a/Documents/TestCases.xlsx
+++ b/Documents/TestCases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="775" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="775" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BUSCADOR DE PASAJEROS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="144">
   <si>
     <t>Indentificador</t>
   </si>
@@ -986,11 +986,6 @@
     <t>No debe permitir seelccionar fechas donde no hayan vuelos (deben mostrar deshabilitadas)</t>
   </si>
   <si>
-    <t>COMO Pasajero
-QUIERO Seleccionar la fecha de ida
-PARA Indicar cuando quiero devolverme</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -999,7 +994,7 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t>QUIERO</t>
+      <t>PARA</t>
     </r>
     <r>
       <rPr>
@@ -1008,7 +1003,7 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Seleccionar la fecha de ida</t>
+      <t xml:space="preserve"> Indicar cuando quiero devolverme</t>
     </r>
   </si>
   <si>
@@ -1020,7 +1015,7 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t>PARA</t>
+      <t>COMO</t>
     </r>
     <r>
       <rPr>
@@ -1029,27 +1024,6 @@
         <rFont val="Segoe UI"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> Indicar cuando quiero devolverme</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>COMO</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF172B4D"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
       <t xml:space="preserve"> Pasajero</t>
     </r>
   </si>
@@ -1058,9 +1032,6 @@
   </si>
   <si>
     <t>Si se selecciona una fecha y la fecha de origen la cambio por una posterior a la fecha de vuelta, la fecha de vuelta se debe eliminar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Destino en el buscador de viajes        </t>
   </si>
   <si>
     <t>Feature: DestinationCity
@@ -1074,6 +1045,106 @@
     Then he can see the destination cities the user can travel to ESPAÑA
 When this user clicks on city of origin
 Then he can select a city from the list of origin cities</t>
+  </si>
+  <si>
+    <t>Feature: DepartureDate
+  As quality control automation
+  I want to enter the departure date
+  Validate departure date selector
+  Background: select departure date
+    Given The user in the search section
+    And this user clicks on the destination city
+  Scenario:Select departure date
+    When choose in the departure date option
+    And the user selects a date enabled
+    Then the lower dates are disabled
+  As QA Automation
+  I want to enter in selector Destination
+  To validate selector Destination
+  Background: Select Selector Destination
+    Given The user in the search section
+  Scenario:Select Selector Destination
+    When this user clicks on destination city
+    Then he can see the destination cities the user can travel to ESPAÑA
+When this user clicks on city of origin
+Then he can select a city from the list of origin cities</t>
+  </si>
+  <si>
+    <t>BUSCADOR FECHA REGRESO</t>
+  </si>
+  <si>
+    <t>COMO Pasajero
+QUIERO Seleccionar la fecha de regreso
+PARA Indicar cuando quiero devolverme</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>QUIERO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Seleccionar la fecha de  regreso</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>QUIERO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF172B4D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Seleccionar la fecha de regreso</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Destino en el buscador de viajes                             3. seleccionamos fecha salida                      4.seleccionamos fecha de regreso</t>
+  </si>
+  <si>
+    <t>Feature: Return Date
+  As quality control automation
+  I want to enter the return date
+  Validate return date selector
+  Background: select return date
+    Given The user in the search section
+    And this user clicks on the destination city
+    And this user clicks start date
+  Scenario: Select return date
+    When choose on the return date
+    And the user changes the checkout date
+    Then user can see later dates disabled
+    And the user selects another departure date, the return date is deselected</t>
+  </si>
+  <si>
+    <t>1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Destino en el buscador de viajes                                 3. Ver Pais y Ciudades de dicho pais</t>
+  </si>
+  <si>
+    <t>1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Origen en el buscador de viajes                             3. seleccionar ciudad de Asturias                                         4. Seleccionar dia 09 del mes de Noviembre                        5.verificar que las fechas inferiores se deshabiliten</t>
+  </si>
+  <si>
+    <t>1. Ir a la URL https://www.volotea.com/es/                                   2. Seleccionar la opcion Origen en el buscador de viajes                             3. seleccionar pestaña Country                                     4.seleccionamos fecha de regreso                                 5. deseleccionar dia de salida</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1364,6 +1435,24 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1490,10 +1579,19 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1864,470 +1962,470 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="34" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="34" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
     </row>
     <row r="4" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="31" t="s">
         <v>38</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="31" t="s">
         <v>88</v>
       </c>
-      <c r="H5" s="25" t="s">
+      <c r="H5" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="26"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="35" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="28" t="s">
+      <c r="H8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="28"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="32" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="25" t="s">
+      <c r="I11" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="25"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="35" t="s">
         <v>38</v>
       </c>
       <c r="D14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="33"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="46" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="32" t="s">
         <v>38</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="26" t="s">
+      <c r="H17" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="25" t="s">
+      <c r="I17" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="25"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="35"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="44" t="s">
         <v>74</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="35" t="s">
         <v>38</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="28" t="s">
+      <c r="G20" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="28" t="s">
+      <c r="H20" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I20" s="28" t="s">
+      <c r="I20" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J20" s="28"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
     </row>
     <row r="22" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="29"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="39" t="s">
+      <c r="B23" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="31" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="H23" s="25" t="s">
+      <c r="H23" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="25"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="35"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="36"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -2935,300 +3033,300 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="60" t="s">
         <v>61</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="54" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="J2" s="52" t="s">
         <v>98</v>
       </c>
       <c r="K2" s="9"/>
     </row>
     <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A3" s="54"/>
+      <c r="A3" s="60"/>
       <c r="B3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="46"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="52"/>
       <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
+      <c r="A4" s="60"/>
       <c r="B4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="46"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="61" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="I5" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="47"/>
+      <c r="J5" s="53"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="52"/>
-      <c r="J6" s="47"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="53"/>
     </row>
     <row r="7" spans="1:11" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="55"/>
+      <c r="A7" s="61"/>
       <c r="B7" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="47"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="59"/>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="53"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="60" t="s">
         <v>62</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="48"/>
+      <c r="J8" s="54"/>
     </row>
     <row r="9" spans="1:11" ht="24" x14ac:dyDescent="0.2">
-      <c r="A9" s="54"/>
+      <c r="A9" s="60"/>
       <c r="B9" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="49"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
-      <c r="J9" s="49"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
     </row>
     <row r="10" spans="1:11" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="54"/>
+      <c r="A10" s="60"/>
       <c r="B10" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
-      <c r="G10" s="50"/>
-      <c r="H10" s="50"/>
-      <c r="I10" s="50"/>
-      <c r="J10" s="50"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="56"/>
+      <c r="J10" s="56"/>
     </row>
     <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="61" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="57" t="s">
         <v>96</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="51" t="s">
+      <c r="F11" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="51" t="s">
+      <c r="H11" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="51" t="s">
+      <c r="I11" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="51"/>
+      <c r="J11" s="57"/>
     </row>
     <row r="12" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="55"/>
+      <c r="A12" s="61"/>
       <c r="B12" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="47"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="52"/>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="52"/>
+      <c r="C12" s="53"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
+      <c r="J12" s="58"/>
     </row>
     <row r="13" spans="1:11" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55"/>
+      <c r="A13" s="61"/>
       <c r="B13" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="47"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="60" t="s">
         <v>65</v>
       </c>
       <c r="B14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="48"/>
+      <c r="J14" s="54"/>
     </row>
     <row r="15" spans="1:11" ht="36" x14ac:dyDescent="0.2">
-      <c r="A15" s="54"/>
+      <c r="A15" s="60"/>
       <c r="B15" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="49"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="55"/>
     </row>
     <row r="16" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="54"/>
+      <c r="A16" s="60"/>
       <c r="B16" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="50"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="50"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
+      <c r="J16" s="56"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
@@ -3444,7 +3542,7 @@
   <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+      <selection activeCell="A2" sqref="A2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3495,360 +3593,360 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="34" t="s">
         <v>109</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="F2" s="56" t="s">
+      <c r="E2" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="F2" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="34"/>
+      <c r="H2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="J2" s="31" t="s">
-        <v>136</v>
+      <c r="J2" s="37" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="32"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="223.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="30"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="33"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="31" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="25" t="s">
+      <c r="E5" s="40"/>
+      <c r="F5" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="32" t="s">
         <v>112</v>
       </c>
-      <c r="J5" s="25"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="26"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="35" t="s">
         <v>109</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="28" t="s">
+      <c r="E8" s="37"/>
+      <c r="F8" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="28" t="s">
+      <c r="I8" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="J8" s="28"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="26"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="51" t="s">
         <v>104</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="29"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="26"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="29"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="29"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="25"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -4359,19 +4457,17 @@
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="I14:I16"/>
     <mergeCell ref="J14:J16"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="J17:J19"/>
     <mergeCell ref="A20:A22"/>
@@ -4383,15 +4479,17 @@
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="I20:I22"/>
     <mergeCell ref="J20:J22"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:J25"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="J23:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -4402,8 +4500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:C19"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4417,7 +4515,7 @@
     <col min="7" max="7" width="32.28515625" style="2" customWidth="1"/>
     <col min="8" max="8" width="12.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="39.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="42.7109375" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -4454,354 +4552,356 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="34" t="s">
         <v>122</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="28" t="s">
+      <c r="E2" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="G2" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="31" t="s">
-        <v>136</v>
+      <c r="J2" s="37" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="67" t="s">
+      <c r="A3" s="51"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="32"/>
-    </row>
-    <row r="4" spans="1:10" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="68" t="s">
+      <c r="E3" s="38"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" spans="1:10" ht="242.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="33"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="31" t="s">
         <v>122</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25" t="s">
+      <c r="G5" s="31"/>
+      <c r="H5" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="25"/>
+      <c r="I5" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="26"/>
+      <c r="A6" s="50"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="27"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="33"/>
       <c r="D7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="51" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="35" t="s">
         <v>122</v>
       </c>
       <c r="D8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="28" t="s">
+      <c r="F8" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28" t="s">
+      <c r="G8" s="34"/>
+      <c r="H8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="J8" s="28"/>
+      <c r="I8" s="34" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:10" ht="33" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="29"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="29"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="29"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -5312,19 +5412,17 @@
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="I14:I16"/>
     <mergeCell ref="J14:J16"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="J17:J19"/>
     <mergeCell ref="A20:A22"/>
@@ -5336,15 +5434,17 @@
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="I20:I22"/>
     <mergeCell ref="J20:J22"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:J25"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="J23:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5354,8 +5454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5406,334 +5506,338 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="51" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="C2" s="28" t="s">
-        <v>38</v>
+      <c r="B2" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>135</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>133</v>
-      </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28" t="s">
+      <c r="E2" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="28" t="s">
-        <v>92</v>
+      <c r="J2" s="34" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="29"/>
+      <c r="A3" s="51"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E3" s="38"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+    </row>
+    <row r="4" spans="1:10" ht="196.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="51"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="39"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="35"/>
+    </row>
+    <row r="5" spans="1:10" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="18" t="s">
         <v>130</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-    </row>
-    <row r="5" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="40" t="s">
+      <c r="E5" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="35"/>
+    </row>
+    <row r="6" spans="1:10" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50"/>
+      <c r="B6" s="46"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="C5" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="E5" s="34" t="s">
-        <v>85</v>
-      </c>
-      <c r="F5" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="25"/>
-    </row>
-    <row r="6" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="E6" s="35"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-    </row>
-    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="33"/>
+      <c r="J7" s="36"/>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="29"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="28"/>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
     </row>
     <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="51"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="29"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="35"/>
+      <c r="H9" s="35"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="35"/>
     </row>
     <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="29"/>
+      <c r="A10" s="51"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="35"/>
       <c r="D10" s="12"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
-      <c r="J10" s="30"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="44"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="26"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="14"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="44"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="26"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="18"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
     </row>
     <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="26"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="32"/>
       <c r="D13" s="14"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
     </row>
     <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="38"/>
-      <c r="C14" s="29"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="11"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
+      <c r="E14" s="37"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="34"/>
     </row>
     <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="45"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="29"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="32"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
     </row>
     <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="29"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="13"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
     </row>
     <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="26"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="18"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="26"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="14"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
     </row>
     <row r="19" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="26"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="15"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33"/>
     </row>
     <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="29"/>
+      <c r="A20" s="51"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="13"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="29"/>
+      <c r="A21" s="51"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="17"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="29"/>
+      <c r="A22" s="51"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="36"/>
     </row>
     <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="44"/>
-      <c r="B23" s="39"/>
-      <c r="C23" s="25"/>
+      <c r="A23" s="50"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="31"/>
       <c r="D23" s="18"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="26"/>
+      <c r="A24" s="50"/>
+      <c r="B24" s="46"/>
+      <c r="C24" s="32"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="27"/>
+      <c r="A25" s="50"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="18"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="33"/>
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="J25" s="33"/>
     </row>
     <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -6204,10 +6308,9 @@
       <c r="J64" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="71">
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="I2:I4"/>
-    <mergeCell ref="J2:J4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="C5:C7"/>
@@ -6222,7 +6325,6 @@
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>
     <mergeCell ref="I5:I7"/>
-    <mergeCell ref="J5:J7"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="C8:C10"/>
@@ -6232,6 +6334,7 @@
     <mergeCell ref="H8:H10"/>
     <mergeCell ref="I8:I10"/>
     <mergeCell ref="J8:J10"/>
+    <mergeCell ref="J2:J7"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
@@ -6244,19 +6347,17 @@
     <mergeCell ref="H14:H16"/>
     <mergeCell ref="I14:I16"/>
     <mergeCell ref="J14:J16"/>
+    <mergeCell ref="G14:G16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="H17:H19"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="F14:F16"/>
-    <mergeCell ref="G14:G16"/>
     <mergeCell ref="I17:I19"/>
     <mergeCell ref="J17:J19"/>
     <mergeCell ref="A20:A22"/>
@@ -6268,15 +6369,17 @@
     <mergeCell ref="H20:H22"/>
     <mergeCell ref="I20:I22"/>
     <mergeCell ref="J20:J22"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="H23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:J25"/>
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="E23:E25"/>
     <mergeCell ref="F23:F25"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="H23:H25"/>
-    <mergeCell ref="I23:I25"/>
-    <mergeCell ref="J23:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6285,10 +6388,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6336,95 +6439,95 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="D2" s="71" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="H2" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="59" t="s">
+      <c r="I2" s="65" t="s">
         <v>46</v>
       </c>
       <c r="J2" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="36" x14ac:dyDescent="0.25">
-      <c r="A3" s="54"/>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="65"/>
+    <row r="3" spans="1:11" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="60"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="71"/>
       <c r="E3" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="60"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="66"/>
       <c r="J3" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="54"/>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="65"/>
+    <row r="4" spans="1:11" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="60"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="72"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="50"/>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="61"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="67"/>
       <c r="J4" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+    <row r="5" spans="1:11" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="69" t="s">
         <v>47</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="62" t="s">
+      <c r="I5" s="68" t="s">
         <v>46</v>
       </c>
       <c r="J5" s="22" t="s">
@@ -6432,56 +6535,327 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="63"/>
+    <row r="6" spans="1:11" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="69"/>
       <c r="E6" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="62"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="68"/>
       <c r="J6" s="22" t="s">
         <v>83</v>
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" ht="54" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="63"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="63"/>
+    <row r="7" spans="1:11" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="61"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="69"/>
       <c r="E7" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="47" t="s">
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="53" t="s">
         <v>84</v>
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="55"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="63"/>
+    <row r="8" spans="1:11" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="61"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="69"/>
       <c r="E8" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="47"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="53"/>
+    </row>
+    <row r="9" spans="1:11" ht="146.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="37" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="37" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="182.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="51"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="38"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="35"/>
+      <c r="H10" s="35"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="38"/>
+    </row>
+    <row r="11" spans="1:11" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="51"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="39"/>
+      <c r="F11" s="64"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="39"/>
+    </row>
+    <row r="12" spans="1:11" ht="174.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="50" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="J12" s="40" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="73" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="76"/>
+      <c r="J13" s="41"/>
+    </row>
+    <row r="14" spans="1:11" ht="167.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="42"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="42"/>
+    </row>
+    <row r="15" spans="1:11" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="J15" s="34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="38"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="35"/>
+    </row>
+    <row r="17" spans="1:10" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="39"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="35"/>
+    </row>
+    <row r="18" spans="1:10" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="H18" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="35"/>
+    </row>
+    <row r="19" spans="1:10" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="50"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="29" t="s">
+        <v>138</v>
+      </c>
+      <c r="E19" s="41"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="35"/>
+    </row>
+    <row r="20" spans="1:10" ht="33" x14ac:dyDescent="0.25">
+      <c r="A20" s="50"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="42"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="77"/>
+      <c r="J20" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="52">
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J20"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="G12:G14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="I12:I14"/>
+    <mergeCell ref="J12:J14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="G9:G11"/>
+    <mergeCell ref="H9:H11"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="G2:G4"/>

</xml_diff>